<commit_message>
Modificacion exitosa de Caja
</commit_message>
<xml_diff>
--- a/11-02-2021.xlsx
+++ b/11-02-2021.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
   <si>
     <t>Reporte de Caja</t>
   </si>
@@ -72,6 +72,15 @@
   </si>
   <si>
     <t>faculoren7@gmail.com</t>
+  </si>
+  <si>
+    <t>2021-02-11 10:54:03.0</t>
+  </si>
+  <si>
+    <t>Egreso</t>
+  </si>
+  <si>
+    <t>2021-02-11 11:21:58.0</t>
   </si>
 </sst>
 </file>
@@ -158,7 +167,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G13"/>
+  <dimension ref="A2:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" zoomScale="150"/>
   </sheetViews>
@@ -336,6 +345,46 @@
         <v>13</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="B2:D3"/>

</xml_diff>